<commit_message>
GPU implementation to be fixed
</commit_message>
<xml_diff>
--- a/TravelingSalesmanProblemQPU/NodesData.xlsx
+++ b/TravelingSalesmanProblemQPU/NodesData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,15 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaime\Documents\reposGitKraken\QuantumProgramming\TravelingSalesmanProblemQPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{075B3744-FBD1-4D74-BEE2-92115E89B276}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49721AF3-968D-4398-86B5-9F9BDF974E29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" activeTab="1"/>
+    <workbookView xWindow="810" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NodesData" sheetId="1" r:id="rId1"/>
     <sheet name="NodesDistances" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -60,7 +71,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -894,12 +905,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:Y21"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:Y21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,11 +998,11 @@
       </c>
       <c r="B2">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1002,79 +1013,79 @@
       </c>
       <c r="G2" cm="1">
         <f t="array" aca="1" ref="G2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>33.120990323358392</v>
+        <v>63.513778032801667</v>
       </c>
       <c r="H2" cm="1">
         <f t="array" aca="1" ref="H2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>80.361682411457764</v>
+        <v>15.556349186104045</v>
       </c>
       <c r="I2" cm="1">
         <f t="array" aca="1" ref="I2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>48.836461788299118</v>
+        <v>63.529520697074361</v>
       </c>
       <c r="J2" cm="1">
         <f t="array" aca="1" ref="J2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>53.535035257296691</v>
+        <v>29.068883707497267</v>
       </c>
       <c r="K2" cm="1">
         <f t="array" aca="1" ref="K2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>34.828149534535996</v>
+        <v>24.331050121192877</v>
       </c>
       <c r="L2" cm="1">
         <f t="array" aca="1" ref="L2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>44.271887242357309</v>
+        <v>90.735880444287304</v>
       </c>
       <c r="M2" cm="1">
         <f t="array" aca="1" ref="M2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>37.363083384538811</v>
+        <v>91.301697684106614</v>
       </c>
       <c r="N2" cm="1">
         <f t="array" aca="1" ref="N2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>102.15674231297707</v>
+        <v>67.683085036070864</v>
       </c>
       <c r="O2" cm="1">
         <f t="array" aca="1" ref="O2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>8.4852813742385695</v>
+        <v>41.785164831552358</v>
       </c>
       <c r="P2" cm="1">
         <f t="array" aca="1" ref="P2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>80.230916734136841</v>
+        <v>33.015148038438355</v>
       </c>
       <c r="Q2" cm="1">
         <f t="array" aca="1" ref="Q2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>21.377558326431949</v>
+        <v>50.487622245457352</v>
       </c>
       <c r="R2" cm="1">
         <f t="array" aca="1" ref="R2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>63.505905237229712</v>
+        <v>76.661594035083823</v>
       </c>
       <c r="S2" cm="1">
         <f t="array" aca="1" ref="S2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>12.083045973594572</v>
+        <v>8.0622577482985491</v>
       </c>
       <c r="T2" cm="1">
         <f t="array" aca="1" ref="T2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>25.45584412271571</v>
+        <v>23.769728648009426</v>
       </c>
       <c r="U2" cm="1">
         <f t="array" aca="1" ref="U2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>89.319650693450427</v>
+        <v>16.763054614240211</v>
       </c>
       <c r="V2" cm="1">
         <f t="array" aca="1" ref="V2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>22.360679774997898</v>
+        <v>38.600518131237564</v>
       </c>
       <c r="W2" cm="1">
         <f t="array" aca="1" ref="W2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>73.545904032787575</v>
+        <v>39.962482405376171</v>
       </c>
       <c r="X2" cm="1">
         <f t="array" aca="1" ref="X2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>36.76955262170047</v>
+        <v>19.209372712298546</v>
       </c>
       <c r="Y2" cm="1">
         <f t="array" aca="1" ref="Y2" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E2),INDEX($C$2:$C$21,$E2),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>58.600341295934449</v>
+        <v>34.014702703389901</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -1083,18 +1094,18 @@
       </c>
       <c r="B3">
         <f t="shared" ref="B3:C21" ca="1" si="0">RANDBETWEEN(0,100)</f>
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" cm="1">
         <f t="array" aca="1" ref="F3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>33.120990323358392</v>
+        <v>63.513778032801667</v>
       </c>
       <c r="G3" cm="1">
         <f t="array" aca="1" ref="G3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
@@ -1102,75 +1113,75 @@
       </c>
       <c r="H3" cm="1">
         <f t="array" aca="1" ref="H3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>80.156097709406993</v>
+        <v>62.289646009589745</v>
       </c>
       <c r="I3" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>37.735924528226413</v>
+        <v>31.144823004794873</v>
       </c>
       <c r="J3" cm="1">
         <f t="array" aca="1" ref="J3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>20.615528128088304</v>
+        <v>55.326304774492215</v>
       </c>
       <c r="K3" cm="1">
         <f t="array" aca="1" ref="K3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>52.172789842982326</v>
+        <v>50.219518117958877</v>
       </c>
       <c r="L3" cm="1">
         <f t="array" aca="1" ref="L3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>13.152946437965905</v>
+        <v>42.296571965113202</v>
       </c>
       <c r="M3" cm="1">
         <f t="array" aca="1" ref="M3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>43.829214001622255</v>
+        <v>45.891175622335062</v>
       </c>
       <c r="N3" cm="1">
         <f t="array" aca="1" ref="N3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>78.771822373231913</v>
+        <v>74.732857566133518</v>
       </c>
       <c r="O3" cm="1">
         <f t="array" aca="1" ref="O3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>36.400549446402593</v>
+        <v>94.148818367518558</v>
       </c>
       <c r="P3" cm="1">
         <f t="array" aca="1" ref="P3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>76.275815302099531</v>
+        <v>93.23089616645332</v>
       </c>
       <c r="Q3" cm="1">
         <f t="array" aca="1" ref="Q3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>51.419840528729765</v>
+        <v>61.846584384264908</v>
       </c>
       <c r="R3" cm="1">
         <f t="array" aca="1" ref="R3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>70.213958726167832</v>
+        <v>34.014702703389901</v>
       </c>
       <c r="S3" cm="1">
         <f t="array" aca="1" ref="S3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>27.658633371878661</v>
+        <v>69.835521047673154</v>
       </c>
       <c r="T3" cm="1">
         <f t="array" aca="1" ref="T3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>47.042533945356304</v>
+        <v>86.95401083331349</v>
       </c>
       <c r="U3" cm="1">
         <f t="array" aca="1" ref="U3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>67.119296778199342</v>
+        <v>79.755877526361658</v>
       </c>
       <c r="V3" cm="1">
         <f t="array" aca="1" ref="V3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>39.204591567825318</v>
+        <v>84.852813742385706</v>
       </c>
       <c r="W3" cm="1">
         <f t="array" aca="1" ref="W3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>57.723478758647246</v>
+        <v>23.600847442411894</v>
       </c>
       <c r="X3" cm="1">
         <f t="array" aca="1" ref="X3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>46.61544808322666</v>
+        <v>60.440052945046304</v>
       </c>
       <c r="Y3" cm="1">
         <f t="array" aca="1" ref="Y3" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E3),INDEX($C$2:$C$21,$E3),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>71.112586790244109</v>
+        <v>30.413812651491099</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
@@ -1179,22 +1190,22 @@
       </c>
       <c r="B4">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" cm="1">
         <f t="array" aca="1" ref="F4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>80.361682411457764</v>
+        <v>15.556349186104045</v>
       </c>
       <c r="G4" cm="1">
         <f t="array" aca="1" ref="G4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>80.156097709406993</v>
+        <v>62.289646009589745</v>
       </c>
       <c r="H4" cm="1">
         <f t="array" aca="1" ref="H4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
@@ -1202,71 +1213,71 @@
       </c>
       <c r="I4" cm="1">
         <f t="array" aca="1" ref="I4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>43.185645763378368</v>
+        <v>69.641941385920603</v>
       </c>
       <c r="J4" cm="1">
         <f t="array" aca="1" ref="J4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>83.234608186739251</v>
+        <v>42.059481689626182</v>
       </c>
       <c r="K4" cm="1">
         <f t="array" aca="1" ref="K4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>50.009999000199947</v>
+        <v>35.693136595149497</v>
       </c>
       <c r="L4" cm="1">
         <f t="array" aca="1" ref="L4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>90.520715861066847</v>
+        <v>95.462034338264544</v>
       </c>
       <c r="M4" cm="1">
         <f t="array" aca="1" ref="M4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>43.011626335213137</v>
+        <v>96.79876032264049</v>
       </c>
       <c r="N4" cm="1">
         <f t="array" aca="1" ref="N4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>65.253352404301808</v>
+        <v>81.271151093115449</v>
       </c>
       <c r="O4" cm="1">
         <f t="array" aca="1" ref="O4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>73.006848993775918</v>
+        <v>56.356011214421486</v>
       </c>
       <c r="P4" cm="1">
         <f t="array" aca="1" ref="P4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>9.2195444572928871</v>
+        <v>45.122056690713912</v>
       </c>
       <c r="Q4" cm="1">
         <f t="array" aca="1" ref="Q4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>73.027392121039071</v>
+        <v>63.600314464631381</v>
       </c>
       <c r="R4" cm="1">
         <f t="array" aca="1" ref="R4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>20.615528128088304</v>
+        <v>81.93289937503738</v>
       </c>
       <c r="S4" cm="1">
         <f t="array" aca="1" ref="S4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>88.76936408468859</v>
+        <v>22.472205054244231</v>
       </c>
       <c r="T4" cm="1">
         <f t="array" aca="1" ref="T4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>59.211485372349848</v>
+        <v>33.060550509633082</v>
       </c>
       <c r="U4" cm="1">
         <f t="array" aca="1" ref="U4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>56.320511361314892</v>
+        <v>27.658633371878661</v>
       </c>
       <c r="V4" cm="1">
         <f t="array" aca="1" ref="V4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>58.463663928973865</v>
+        <v>54.037024344425184</v>
       </c>
       <c r="W4" cm="1">
         <f t="array" aca="1" ref="W4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>38.327535793473601</v>
+        <v>39.408120990476064</v>
       </c>
       <c r="X4" cm="1">
         <f t="array" aca="1" ref="X4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>43.931765272977593</v>
+        <v>4.1231056256176606</v>
       </c>
       <c r="Y4" cm="1">
         <f t="array" aca="1" ref="Y4" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E4),INDEX($C$2:$C$21,$E4),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>32.310988842807021</v>
+        <v>32.015621187164243</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
@@ -1275,26 +1286,26 @@
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" cm="1">
         <f t="array" aca="1" ref="F5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>48.836461788299118</v>
+        <v>63.529520697074361</v>
       </c>
       <c r="G5" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>37.735924528226413</v>
+        <v>31.144823004794873</v>
       </c>
       <c r="H5" cm="1">
         <f t="array" aca="1" ref="H5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>43.185645763378368</v>
+        <v>69.641941385920603</v>
       </c>
       <c r="I5" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
@@ -1302,67 +1313,67 @@
       </c>
       <c r="J5" cm="1">
         <f t="array" aca="1" ref="J5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>40.70626487409524</v>
+        <v>41.868842830916641</v>
       </c>
       <c r="K5" cm="1">
         <f t="array" aca="1" ref="K5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>37.443290453698111</v>
+        <v>41.231056256176608</v>
       </c>
       <c r="L5" cm="1">
         <f t="array" aca="1" ref="L5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>47.381430961928537</v>
+        <v>27.658633371878661</v>
       </c>
       <c r="M5" cm="1">
         <f t="array" aca="1" ref="M5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>22.472205054244231</v>
+        <v>27.784887978899608</v>
       </c>
       <c r="N5" cm="1">
         <f t="array" aca="1" ref="N5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>55.470712993434653</v>
+        <v>46.097722286464439</v>
       </c>
       <c r="O5" cm="1">
         <f t="array" aca="1" ref="O5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>44.598206241955516</v>
+        <v>80.262070743284468</v>
       </c>
       <c r="P5" cm="1">
         <f t="array" aca="1" ref="P5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>38.600518131237564</v>
+        <v>84.958813551037778</v>
       </c>
       <c r="Q5" cm="1">
         <f t="array" aca="1" ref="Q5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>53.254107822777392</v>
+        <v>37.483329627982627</v>
       </c>
       <c r="R5" cm="1">
         <f t="array" aca="1" ref="R5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>38.078865529319543</v>
+        <v>13.45362404707371</v>
       </c>
       <c r="S5" cm="1">
         <f t="array" aca="1" ref="S5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>53.037722424704477</v>
+        <v>66.850579653433073</v>
       </c>
       <c r="T5" cm="1">
         <f t="array" aca="1" ref="T5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>40.36087214122113</v>
+        <v>83.240615086627031</v>
       </c>
       <c r="U5" cm="1">
         <f t="array" aca="1" ref="U5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>42.43819034784589</v>
+        <v>76.400261779656233</v>
       </c>
       <c r="V5" cm="1">
         <f t="array" aca="1" ref="V5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>33.837848631377263</v>
+        <v>69.354163537598808</v>
       </c>
       <c r="W5" cm="1">
         <f t="array" aca="1" ref="W5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>24.738633753705962</v>
+        <v>35.227829907617071</v>
       </c>
       <c r="X5" cm="1">
         <f t="array" aca="1" ref="X5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>26.92582403567252</v>
+        <v>69.634761434214738</v>
       </c>
       <c r="Y5" cm="1">
         <f t="array" aca="1" ref="Y5" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E5),INDEX($C$2:$C$21,$E5),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>44.011362169330773</v>
+        <v>42.01190307520001</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
@@ -1371,30 +1382,30 @@
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="0"/>
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>89</v>
+        <v>43</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>53.535035257296691</v>
+        <v>29.068883707497267</v>
       </c>
       <c r="G6" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>20.615528128088304</v>
+        <v>55.326304774492215</v>
       </c>
       <c r="H6" cm="1">
         <f t="array" aca="1" ref="H6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>83.234608186739251</v>
+        <v>42.059481689626182</v>
       </c>
       <c r="I6" cm="1">
         <f t="array" aca="1" ref="I6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>40.70626487409524</v>
+        <v>41.868842830916641</v>
       </c>
       <c r="J6" cm="1">
         <f t="array" aca="1" ref="J6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
@@ -1402,63 +1413,63 @@
       </c>
       <c r="K6" cm="1">
         <f t="array" aca="1" ref="K6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>67.029844099475568</v>
+        <v>7.810249675906654</v>
       </c>
       <c r="L6" cm="1">
         <f t="array" aca="1" ref="L6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>15.297058540778355</v>
+        <v>69.31089380465383</v>
       </c>
       <c r="M6" cm="1">
         <f t="array" aca="1" ref="M6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>55.443665102516448</v>
+        <v>68.680419334771102</v>
       </c>
       <c r="N6" cm="1">
         <f t="array" aca="1" ref="N6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>65.192024052026483</v>
+        <v>39.217343102255157</v>
       </c>
       <c r="O6" cm="1">
         <f t="array" aca="1" ref="O6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>55.946402922797461</v>
+        <v>39.560080889704963</v>
       </c>
       <c r="P6" cm="1">
         <f t="array" aca="1" ref="P6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>77.336925203941234</v>
+        <v>43.139309220245984</v>
       </c>
       <c r="Q6" cm="1">
         <f t="array" aca="1" ref="Q6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>70.576199954375554</v>
+        <v>21.587033144922902</v>
       </c>
       <c r="R6" cm="1">
         <f t="array" aca="1" ref="R6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>78.185676437567508</v>
+        <v>55.226805085936306</v>
       </c>
       <c r="S6" cm="1">
         <f t="array" aca="1" ref="S6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>48.083261120685229</v>
+        <v>28.635642126552707</v>
       </c>
       <c r="T6" cm="1">
         <f t="array" aca="1" ref="T6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>63.953107821277925</v>
+        <v>42.941821107167776</v>
       </c>
       <c r="U6" cm="1">
         <f t="array" aca="1" ref="U6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>55.317266743757322</v>
+        <v>36.76955262170047</v>
       </c>
       <c r="V6" cm="1">
         <f t="array" aca="1" ref="V6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>55.731499172371095</v>
+        <v>29.614185789921695</v>
       </c>
       <c r="W6" cm="1">
         <f t="array" aca="1" ref="W6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>52.430906915673319</v>
+        <v>36.878177829171548</v>
       </c>
       <c r="X6" cm="1">
         <f t="array" aca="1" ref="X6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>59.211485372349848</v>
+        <v>44.384682042344295</v>
       </c>
       <c r="Y6" cm="1">
         <f t="array" aca="1" ref="Y6" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E6),INDEX($C$2:$C$21,$E6),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>82</v>
+        <v>36.249137920783717</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.25">
@@ -1467,34 +1478,34 @@
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>42</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" cm="1">
         <f t="array" aca="1" ref="F7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>34.828149534535996</v>
+        <v>24.331050121192877</v>
       </c>
       <c r="G7" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>52.172789842982326</v>
+        <v>50.219518117958877</v>
       </c>
       <c r="H7" cm="1">
         <f t="array" aca="1" ref="H7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>50.009999000199947</v>
+        <v>35.693136595149497</v>
       </c>
       <c r="I7" cm="1">
         <f t="array" aca="1" ref="I7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>37.443290453698111</v>
+        <v>41.231056256176608</v>
       </c>
       <c r="J7" cm="1">
         <f t="array" aca="1" ref="J7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>67.029844099475568</v>
+        <v>7.810249675906654</v>
       </c>
       <c r="K7" cm="1">
         <f t="array" aca="1" ref="K7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
@@ -1502,59 +1513,59 @@
       </c>
       <c r="L7" cm="1">
         <f t="array" aca="1" ref="L7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>65.30696746902278</v>
+        <v>68.8839603971781</v>
       </c>
       <c r="M7" cm="1">
         <f t="array" aca="1" ref="M7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>15</v>
+        <v>68.818602136341013</v>
       </c>
       <c r="N7" cm="1">
         <f t="array" aca="1" ref="N7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>91.285267157411553</v>
+        <v>46.097722286464439</v>
       </c>
       <c r="O7" cm="1">
         <f t="array" aca="1" ref="O7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>26.40075756488817</v>
+        <v>43.931765272977593</v>
       </c>
       <c r="P7" cm="1">
         <f t="array" aca="1" ref="P7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>52.611785751863621</v>
+        <v>44.654227123532216</v>
       </c>
       <c r="Q7" cm="1">
         <f t="array" aca="1" ref="Q7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>23.021728866442675</v>
+        <v>28.231188426986208</v>
       </c>
       <c r="R7" cm="1">
         <f t="array" aca="1" ref="R7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>30.594117081556711</v>
+        <v>54.671747731346578</v>
       </c>
       <c r="S7" cm="1">
         <f t="array" aca="1" ref="S7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>45.967379738244816</v>
+        <v>25.942243542145693</v>
       </c>
       <c r="T7" cm="1">
         <f t="array" aca="1" ref="T7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>9.8488578017961039</v>
+        <v>42.01190307520001</v>
       </c>
       <c r="U7" cm="1">
         <f t="array" aca="1" ref="U7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>78.492037812761623</v>
+        <v>35.227829907617071</v>
       </c>
       <c r="V7" cm="1">
         <f t="array" aca="1" ref="V7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>13.892443989449804</v>
+        <v>35.014282800023196</v>
       </c>
       <c r="W7" cm="1">
         <f t="array" aca="1" ref="W7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>58.258046654518033</v>
+        <v>30.14962686336267</v>
       </c>
       <c r="X7" cm="1">
         <f t="array" aca="1" ref="X7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>10.63014581273465</v>
+        <v>37.643060449437421</v>
       </c>
       <c r="Y7" cm="1">
         <f t="array" aca="1" ref="Y7" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E7),INDEX($C$2:$C$21,$E7),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>23.853720883753127</v>
+        <v>28.792360097775937</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
@@ -1563,38 +1574,38 @@
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="0"/>
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
       <c r="F8" cm="1">
         <f t="array" aca="1" ref="F8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>44.271887242357309</v>
+        <v>90.735880444287304</v>
       </c>
       <c r="G8" cm="1">
         <f t="array" aca="1" ref="G8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>13.152946437965905</v>
+        <v>42.296571965113202</v>
       </c>
       <c r="H8" cm="1">
         <f t="array" aca="1" ref="H8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>90.520715861066847</v>
+        <v>95.462034338264544</v>
       </c>
       <c r="I8" cm="1">
         <f t="array" aca="1" ref="I8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>47.381430961928537</v>
+        <v>27.658633371878661</v>
       </c>
       <c r="J8" cm="1">
         <f t="array" aca="1" ref="J8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>15.297058540778355</v>
+        <v>69.31089380465383</v>
       </c>
       <c r="K8" cm="1">
         <f t="array" aca="1" ref="K8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>65.30696746902278</v>
+        <v>68.8839603971781</v>
       </c>
       <c r="L8" cm="1">
         <f t="array" aca="1" ref="L8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
@@ -1602,55 +1613,55 @@
       </c>
       <c r="M8" cm="1">
         <f t="array" aca="1" ref="M8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>56.462376853972415</v>
+        <v>5</v>
       </c>
       <c r="N8" cm="1">
         <f t="array" aca="1" ref="N8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>80.02499609497022</v>
+        <v>63.953107821277925</v>
       </c>
       <c r="O8" cm="1">
         <f t="array" aca="1" ref="O8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>48.662100242385755</v>
+        <v>106.83164325236227</v>
       </c>
       <c r="P8" cm="1">
         <f t="array" aca="1" ref="P8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>85.796270315206598</v>
+        <v>112.44998888394787</v>
       </c>
       <c r="Q8" cm="1">
         <f t="array" aca="1" ref="Q8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>63.788713735268246</v>
+        <v>61.26989472816156</v>
       </c>
       <c r="R8" cm="1">
         <f t="array" aca="1" ref="R8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>82.152297594163485</v>
+        <v>14.212670403551895</v>
       </c>
       <c r="S8" cm="1">
         <f t="array" aca="1" ref="S8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>36.359317925395686</v>
+        <v>94.403389769647575</v>
       </c>
       <c r="T8" cm="1">
         <f t="array" aca="1" ref="T8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>60.133185513491632</v>
+        <v>110.8873302050329</v>
       </c>
       <c r="U8" cm="1">
         <f t="array" aca="1" ref="U8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>69.584481028459209</v>
+        <v>104.01922899156675</v>
       </c>
       <c r="V8" cm="1">
         <f t="array" aca="1" ref="V8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>52.345009313209601</v>
+        <v>95.692214939356489</v>
       </c>
       <c r="W8" cm="1">
         <f t="array" aca="1" ref="W8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>63.976558206893252</v>
+        <v>57.723478758647246</v>
       </c>
       <c r="X8" cm="1">
         <f t="array" aca="1" ref="X8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>59.464274989274024</v>
+        <v>94.921019800674287</v>
       </c>
       <c r="Y8" cm="1">
         <f t="array" aca="1" ref="Y8" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E8),INDEX($C$2:$C$21,$E8),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>83.773504164502995</v>
+        <v>65.253352404301808</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
@@ -1659,42 +1670,42 @@
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="0"/>
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>89</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
       <c r="F9" cm="1">
         <f t="array" aca="1" ref="F9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>37.363083384538811</v>
+        <v>91.301697684106614</v>
       </c>
       <c r="G9" cm="1">
         <f t="array" aca="1" ref="G9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>43.829214001622255</v>
+        <v>45.891175622335062</v>
       </c>
       <c r="H9" cm="1">
         <f t="array" aca="1" ref="H9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>43.011626335213137</v>
+        <v>96.79876032264049</v>
       </c>
       <c r="I9" cm="1">
         <f t="array" aca="1" ref="I9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>22.472205054244231</v>
+        <v>27.784887978899608</v>
       </c>
       <c r="J9" cm="1">
         <f t="array" aca="1" ref="J9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>55.443665102516448</v>
+        <v>68.680419334771102</v>
       </c>
       <c r="K9" cm="1">
         <f t="array" aca="1" ref="K9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>15</v>
+        <v>68.818602136341013</v>
       </c>
       <c r="L9" cm="1">
         <f t="array" aca="1" ref="L9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>56.462376853972415</v>
+        <v>5</v>
       </c>
       <c r="M9" cm="1">
         <f t="array" aca="1" ref="M9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
@@ -1702,51 +1713,51 @@
       </c>
       <c r="N9" cm="1">
         <f t="array" aca="1" ref="N9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>76.576758876306585</v>
+        <v>60.638271743182131</v>
       </c>
       <c r="O9" cm="1">
         <f t="array" aca="1" ref="O9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>30.265491900843113</v>
+        <v>105.42295765154761</v>
       </c>
       <c r="P9" cm="1">
         <f t="array" aca="1" ref="P9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>43.185645763378368</v>
+        <v>111.75866856758807</v>
       </c>
       <c r="Q9" cm="1">
         <f t="array" aca="1" ref="Q9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>33.837848631377263</v>
+        <v>59.169248769948062</v>
       </c>
       <c r="R9" cm="1">
         <f t="array" aca="1" ref="R9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>27.658633371878661</v>
+        <v>14.866068747318506</v>
       </c>
       <c r="S9" cm="1">
         <f t="array" aca="1" ref="S9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>46.065171225124082</v>
+        <v>94.578010129204984</v>
       </c>
       <c r="T9" cm="1">
         <f t="array" aca="1" ref="T9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>19.697715603592208</v>
+        <v>110.80162453682708</v>
       </c>
       <c r="U9" cm="1">
         <f t="array" aca="1" ref="U9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>63.702433234531945</v>
+        <v>104.04326023342406</v>
       </c>
       <c r="V9" cm="1">
         <f t="array" aca="1" ref="V9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>16</v>
+        <v>94.201910808645493</v>
       </c>
       <c r="W9" cm="1">
         <f t="array" aca="1" ref="W9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>43.829214001622255</v>
+        <v>59.841457201508724</v>
       </c>
       <c r="X9" cm="1">
         <f t="array" aca="1" ref="X9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>4.4721359549995796</v>
+        <v>96.462427918853464</v>
       </c>
       <c r="Y9" cm="1">
         <f t="array" aca="1" ref="Y9" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E9),INDEX($C$2:$C$21,$E9),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>27.313000567495326</v>
+        <v>67.268120235368556</v>
       </c>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
@@ -1755,46 +1766,46 @@
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>84</v>
+        <v>30</v>
       </c>
       <c r="E10">
         <v>9</v>
       </c>
       <c r="F10" cm="1">
         <f t="array" aca="1" ref="F10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>102.15674231297707</v>
+        <v>67.683085036070864</v>
       </c>
       <c r="G10" cm="1">
         <f t="array" aca="1" ref="G10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>78.771822373231913</v>
+        <v>74.732857566133518</v>
       </c>
       <c r="H10" cm="1">
         <f t="array" aca="1" ref="H10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>65.253352404301808</v>
+        <v>81.271151093115449</v>
       </c>
       <c r="I10" cm="1">
         <f t="array" aca="1" ref="I10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>55.470712993434653</v>
+        <v>46.097722286464439</v>
       </c>
       <c r="J10" cm="1">
         <f t="array" aca="1" ref="J10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>65.192024052026483</v>
+        <v>39.217343102255157</v>
       </c>
       <c r="K10" cm="1">
         <f t="array" aca="1" ref="K10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>91.285267157411553</v>
+        <v>46.097722286464439</v>
       </c>
       <c r="L10" cm="1">
         <f t="array" aca="1" ref="L10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>80.02499609497022</v>
+        <v>63.953107821277925</v>
       </c>
       <c r="M10" cm="1">
         <f t="array" aca="1" ref="M10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>76.576758876306585</v>
+        <v>60.638271743182131</v>
       </c>
       <c r="N10" cm="1">
         <f t="array" aca="1" ref="N10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
@@ -1802,47 +1813,47 @@
       </c>
       <c r="O10" cm="1">
         <f t="array" aca="1" ref="O10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>99.297532698451278</v>
+        <v>56.36488268416781</v>
       </c>
       <c r="P10" cm="1">
         <f t="array" aca="1" ref="P10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>56.044625076808217</v>
+        <v>69.375788283809797</v>
       </c>
       <c r="Q10" cm="1">
         <f t="array" aca="1" ref="Q10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>108.72442227944924</v>
+        <v>17.888543819998318</v>
       </c>
       <c r="R10" cm="1">
         <f t="array" aca="1" ref="R10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>77.414468931847622</v>
+        <v>54</v>
       </c>
       <c r="S10" cm="1">
         <f t="array" aca="1" ref="S10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>103.16006979447037</v>
+        <v>65.375836514724611</v>
       </c>
       <c r="T10" cm="1">
         <f t="array" aca="1" ref="T10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>95.603347221736954</v>
+        <v>75.325958341065927</v>
       </c>
       <c r="U10" cm="1">
         <f t="array" aca="1" ref="U10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>13.038404810405298</v>
+        <v>71.007041904306931</v>
       </c>
       <c r="V10" cm="1">
         <f t="array" aca="1" ref="V10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>89.308454247064432</v>
+        <v>45.880278987817846</v>
       </c>
       <c r="W10" cm="1">
         <f t="array" aca="1" ref="W10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>33.301651610693426</v>
+        <v>66.528189513919585</v>
       </c>
       <c r="X10" cm="1">
         <f t="array" aca="1" ref="X10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>80.721744282442259</v>
+        <v>83.570329663104715</v>
       </c>
       <c r="Y10" cm="1">
         <f t="array" aca="1" ref="Y10" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E10),INDEX($C$2:$C$21,$E10),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>88.509886453435243</v>
+        <v>69.426219830839131</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
@@ -1851,50 +1862,50 @@
       </c>
       <c r="B11">
         <f t="shared" ca="1" si="0"/>
-        <v>88</v>
+        <v>33</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>38</v>
+        <v>6</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11" cm="1">
         <f t="array" aca="1" ref="F11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>8.4852813742385695</v>
+        <v>41.785164831552358</v>
       </c>
       <c r="G11" cm="1">
         <f t="array" aca="1" ref="G11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>36.400549446402593</v>
+        <v>94.148818367518558</v>
       </c>
       <c r="H11" cm="1">
         <f t="array" aca="1" ref="H11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>73.006848993775918</v>
+        <v>56.356011214421486</v>
       </c>
       <c r="I11" cm="1">
         <f t="array" aca="1" ref="I11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>44.598206241955516</v>
+        <v>80.262070743284468</v>
       </c>
       <c r="J11" cm="1">
         <f t="array" aca="1" ref="J11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>55.946402922797461</v>
+        <v>39.560080889704963</v>
       </c>
       <c r="K11" cm="1">
         <f t="array" aca="1" ref="K11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>26.40075756488817</v>
+        <v>43.931765272977593</v>
       </c>
       <c r="L11" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>48.662100242385755</v>
+        <v>106.83164325236227</v>
       </c>
       <c r="M11" cm="1">
         <f t="array" aca="1" ref="M11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>30.265491900843113</v>
+        <v>105.42295765154761</v>
       </c>
       <c r="N11" cm="1">
         <f t="array" aca="1" ref="N11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>99.297532698451278</v>
+        <v>56.36488268416781</v>
       </c>
       <c r="O11" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
@@ -1902,43 +1913,43 @@
       </c>
       <c r="P11" cm="1">
         <f t="array" aca="1" ref="P11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>73.437047870948632</v>
+        <v>17.088007490635061</v>
       </c>
       <c r="Q11" cm="1">
         <f t="array" aca="1" ref="Q11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>15.132745950421556</v>
+        <v>47.423622805517503</v>
       </c>
       <c r="R11" cm="1">
         <f t="array" aca="1" ref="R11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>55.542776307995261</v>
+        <v>93.1933474020544</v>
       </c>
       <c r="S11" cm="1">
         <f t="array" aca="1" ref="S11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>20.248456731316587</v>
+        <v>34.014702703389901</v>
       </c>
       <c r="T11" cm="1">
         <f t="array" aca="1" ref="T11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>16.970562748477139</v>
+        <v>29.410882339705484</v>
       </c>
       <c r="U11" cm="1">
         <f t="array" aca="1" ref="U11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>86.313382508160345</v>
+        <v>30.479501308256342</v>
       </c>
       <c r="V11" cm="1">
         <f t="array" aca="1" ref="V11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>14.560219778561036</v>
+        <v>11.313708498984761</v>
       </c>
       <c r="W11" cm="1">
         <f t="array" aca="1" ref="W11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>69.260378283691168</v>
+        <v>73.246160308919954</v>
       </c>
       <c r="X11" cm="1">
         <f t="array" aca="1" ref="X11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>29.120439557122072</v>
+        <v>60.373835392494321</v>
       </c>
       <c r="Y11" cm="1">
         <f t="array" aca="1" ref="Y11" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E11),INDEX($C$2:$C$21,$E11),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>50.219518117958877</v>
+        <v>70.007142492748557</v>
       </c>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
@@ -1947,54 +1958,54 @@
       </c>
       <c r="B12">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E12">
         <v>11</v>
       </c>
       <c r="F12" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>80.230916734136841</v>
+        <v>33.015148038438355</v>
       </c>
       <c r="G12" cm="1">
         <f t="array" aca="1" ref="G12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>76.275815302099531</v>
+        <v>93.23089616645332</v>
       </c>
       <c r="H12" cm="1">
         <f t="array" aca="1" ref="H12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>9.2195444572928871</v>
+        <v>45.122056690713912</v>
       </c>
       <c r="I12" cm="1">
         <f t="array" aca="1" ref="I12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>38.600518131237564</v>
+        <v>84.958813551037778</v>
       </c>
       <c r="J12" cm="1">
         <f t="array" aca="1" ref="J12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>77.336925203941234</v>
+        <v>43.139309220245984</v>
       </c>
       <c r="K12" cm="1">
         <f t="array" aca="1" ref="K12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>52.611785751863621</v>
+        <v>44.654227123532216</v>
       </c>
       <c r="L12" cm="1">
         <f t="array" aca="1" ref="L12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>85.796270315206598</v>
+        <v>112.44998888394787</v>
       </c>
       <c r="M12" cm="1">
         <f t="array" aca="1" ref="M12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>43.185645763378368</v>
+        <v>111.75866856758807</v>
       </c>
       <c r="N12" cm="1">
         <f t="array" aca="1" ref="N12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>56.044625076808217</v>
+        <v>69.375788283809797</v>
       </c>
       <c r="O12" cm="1">
         <f t="array" aca="1" ref="O12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>73.437047870948632</v>
+        <v>17.088007490635061</v>
       </c>
       <c r="P12" cm="1">
         <f t="array" aca="1" ref="P12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
@@ -2002,39 +2013,39 @@
       </c>
       <c r="Q12" cm="1">
         <f t="array" aca="1" ref="Q12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>75.325958341065927</v>
+        <v>57.245087125446844</v>
       </c>
       <c r="R12" cm="1">
         <f t="array" aca="1" ref="R12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>26.076809620810597</v>
+        <v>98.35141076771599</v>
       </c>
       <c r="S12" cm="1">
         <f t="array" aca="1" ref="S12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>87.641314458421945</v>
+        <v>25.079872407968907</v>
       </c>
       <c r="T12" cm="1">
         <f t="array" aca="1" ref="T12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>61.1310068623117</v>
+        <v>13.601470508735444</v>
       </c>
       <c r="U12" cm="1">
         <f t="array" aca="1" ref="U12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>47.169905660283021</v>
+        <v>17.464249196572979</v>
       </c>
       <c r="V12" cm="1">
         <f t="array" aca="1" ref="V12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>59.135437767890075</v>
+        <v>24.083189157584592</v>
       </c>
       <c r="W12" cm="1">
         <f t="array" aca="1" ref="W12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>29.832867780352597</v>
+        <v>70.51950084905593</v>
       </c>
       <c r="X12" cm="1">
         <f t="array" aca="1" ref="X12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>45</v>
+        <v>49.244289008980523</v>
       </c>
       <c r="Y12" cm="1">
         <f t="array" aca="1" ref="Y12" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E12),INDEX($C$2:$C$21,$E12),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>38.275318418009277</v>
+        <v>65.73431371817918</v>
       </c>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
@@ -2043,58 +2054,58 @@
       </c>
       <c r="B13">
         <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="E13">
         <v>12</v>
       </c>
       <c r="F13" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>21.377558326431949</v>
+        <v>50.487622245457352</v>
       </c>
       <c r="G13" cm="1">
         <f t="array" aca="1" ref="G13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>51.419840528729765</v>
+        <v>61.846584384264908</v>
       </c>
       <c r="H13" cm="1">
         <f t="array" aca="1" ref="H13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>73.027392121039071</v>
+        <v>63.600314464631381</v>
       </c>
       <c r="I13" cm="1">
         <f t="array" aca="1" ref="I13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>53.254107822777392</v>
+        <v>37.483329627982627</v>
       </c>
       <c r="J13" cm="1">
         <f t="array" aca="1" ref="J13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>70.576199954375554</v>
+        <v>21.587033144922902</v>
       </c>
       <c r="K13" cm="1">
         <f t="array" aca="1" ref="K13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>23.021728866442675</v>
+        <v>28.231188426986208</v>
       </c>
       <c r="L13" cm="1">
         <f t="array" aca="1" ref="L13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>63.788713735268246</v>
+        <v>61.26989472816156</v>
       </c>
       <c r="M13" cm="1">
         <f t="array" aca="1" ref="M13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>33.837848631377263</v>
+        <v>59.169248769948062</v>
       </c>
       <c r="N13" cm="1">
         <f t="array" aca="1" ref="N13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>108.72442227944924</v>
+        <v>17.888543819998318</v>
       </c>
       <c r="O13" cm="1">
         <f t="array" aca="1" ref="O13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>15.132745950421556</v>
+        <v>47.423622805517503</v>
       </c>
       <c r="P13" cm="1">
         <f t="array" aca="1" ref="P13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>75.325958341065927</v>
+        <v>57.245087125446844</v>
       </c>
       <c r="Q13" cm="1">
         <f t="array" aca="1" ref="Q13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
@@ -2102,35 +2113,35 @@
       </c>
       <c r="R13" cm="1">
         <f t="array" aca="1" ref="R13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>53.460265618494638</v>
+        <v>48.703182647543684</v>
       </c>
       <c r="S13" cm="1">
         <f t="array" aca="1" ref="S13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>33.241540277189323</v>
+        <v>49.010203019371382</v>
       </c>
       <c r="T13" cm="1">
         <f t="array" aca="1" ref="T13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>14.317821063276353</v>
+        <v>60.876925020897694</v>
       </c>
       <c r="U13" cm="1">
         <f t="array" aca="1" ref="U13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>95.692214939356489</v>
+        <v>55.731499172371095</v>
       </c>
       <c r="V13" cm="1">
         <f t="array" aca="1" ref="V13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>19.416487838947599</v>
+        <v>36.124783736376884</v>
       </c>
       <c r="W13" cm="1">
         <f t="array" aca="1" ref="W13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>76.941536246685374</v>
+        <v>50.219518117958877</v>
       </c>
       <c r="X13" cm="1">
         <f t="array" aca="1" ref="X13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>30.805843601498726</v>
+        <v>65.787536813594102</v>
       </c>
       <c r="Y13" cm="1">
         <f t="array" aca="1" ref="Y13" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E13),INDEX($C$2:$C$21,$E13),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>45.221676218380054</v>
+        <v>52.345009313209601</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
@@ -2139,62 +2150,62 @@
       </c>
       <c r="B14">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>84</v>
       </c>
       <c r="E14">
         <v>13</v>
       </c>
       <c r="F14" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>63.505905237229712</v>
+        <v>76.661594035083823</v>
       </c>
       <c r="G14" cm="1">
         <f t="array" aca="1" ref="G14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>70.213958726167832</v>
+        <v>34.014702703389901</v>
       </c>
       <c r="H14" cm="1">
         <f t="array" aca="1" ref="H14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>20.615528128088304</v>
+        <v>81.93289937503738</v>
       </c>
       <c r="I14" cm="1">
         <f t="array" aca="1" ref="I14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>38.078865529319543</v>
+        <v>13.45362404707371</v>
       </c>
       <c r="J14" cm="1">
         <f t="array" aca="1" ref="J14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>78.185676437567508</v>
+        <v>55.226805085936306</v>
       </c>
       <c r="K14" cm="1">
         <f t="array" aca="1" ref="K14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>30.594117081556711</v>
+        <v>54.671747731346578</v>
       </c>
       <c r="L14" cm="1">
         <f t="array" aca="1" ref="L14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>82.152297594163485</v>
+        <v>14.212670403551895</v>
       </c>
       <c r="M14" cm="1">
         <f t="array" aca="1" ref="M14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>27.658633371878661</v>
+        <v>14.866068747318506</v>
       </c>
       <c r="N14" cm="1">
         <f t="array" aca="1" ref="N14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>77.414468931847622</v>
+        <v>54</v>
       </c>
       <c r="O14" cm="1">
         <f t="array" aca="1" ref="O14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>55.542776307995261</v>
+        <v>93.1933474020544</v>
       </c>
       <c r="P14" cm="1">
         <f t="array" aca="1" ref="P14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>26.076809620810597</v>
+        <v>98.35141076771599</v>
       </c>
       <c r="Q14" cm="1">
         <f t="array" aca="1" ref="Q14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>53.460265618494638</v>
+        <v>48.703182647543684</v>
       </c>
       <c r="R14" cm="1">
         <f t="array" aca="1" ref="R14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
@@ -2202,31 +2213,31 @@
       </c>
       <c r="S14" cm="1">
         <f t="array" aca="1" ref="S14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>73.246160308919954</v>
+        <v>80.212218520621903</v>
       </c>
       <c r="T14" cm="1">
         <f t="array" aca="1" ref="T14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>40.26164427839479</v>
+        <v>96.674712308855618</v>
       </c>
       <c r="U14" cm="1">
         <f t="array" aca="1" ref="U14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>66.309878600401618</v>
+        <v>89.810912477270818</v>
       </c>
       <c r="V14" cm="1">
         <f t="array" aca="1" ref="V14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>41.146081222881968</v>
+        <v>82.152297594163485</v>
       </c>
       <c r="W14" cm="1">
         <f t="array" aca="1" ref="W14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>45.541190146942803</v>
+        <v>45.276925690687087</v>
       </c>
       <c r="X14" cm="1">
         <f t="array" aca="1" ref="X14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>26.92582403567252</v>
+        <v>81.60882305241266</v>
       </c>
       <c r="Y14" cm="1">
         <f t="array" aca="1" ref="Y14" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E14),INDEX($C$2:$C$21,$E14),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>12.206555615733702</v>
+        <v>52.611785751863621</v>
       </c>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
@@ -2235,66 +2246,66 @@
       </c>
       <c r="B15">
         <f t="shared" ca="1" si="0"/>
-        <v>99</v>
+        <v>19</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>37</v>
       </c>
       <c r="E15">
         <v>14</v>
       </c>
       <c r="F15" cm="1">
         <f t="array" aca="1" ref="F15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>12.083045973594572</v>
+        <v>8.0622577482985491</v>
       </c>
       <c r="G15" cm="1">
         <f t="array" aca="1" ref="G15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>27.658633371878661</v>
+        <v>69.835521047673154</v>
       </c>
       <c r="H15" cm="1">
         <f t="array" aca="1" ref="H15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>88.76936408468859</v>
+        <v>22.472205054244231</v>
       </c>
       <c r="I15" cm="1">
         <f t="array" aca="1" ref="I15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>53.037722424704477</v>
+        <v>66.850579653433073</v>
       </c>
       <c r="J15" cm="1">
         <f t="array" aca="1" ref="J15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>48.083261120685229</v>
+        <v>28.635642126552707</v>
       </c>
       <c r="K15" cm="1">
         <f t="array" aca="1" ref="K15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>45.967379738244816</v>
+        <v>25.942243542145693</v>
       </c>
       <c r="L15" cm="1">
         <f t="array" aca="1" ref="L15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>36.359317925395686</v>
+        <v>94.403389769647575</v>
       </c>
       <c r="M15" cm="1">
         <f t="array" aca="1" ref="M15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>46.065171225124082</v>
+        <v>94.578010129204984</v>
       </c>
       <c r="N15" cm="1">
         <f t="array" aca="1" ref="N15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>103.16006979447037</v>
+        <v>65.375836514724611</v>
       </c>
       <c r="O15" cm="1">
         <f t="array" aca="1" ref="O15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>20.248456731316587</v>
+        <v>34.014702703389901</v>
       </c>
       <c r="P15" cm="1">
         <f t="array" aca="1" ref="P15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>87.641314458421945</v>
+        <v>25.079872407968907</v>
       </c>
       <c r="Q15" cm="1">
         <f t="array" aca="1" ref="Q15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>33.241540277189323</v>
+        <v>49.010203019371382</v>
       </c>
       <c r="R15" cm="1">
         <f t="array" aca="1" ref="R15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>73.246160308919954</v>
+        <v>80.212218520621903</v>
       </c>
       <c r="S15" cm="1">
         <f t="array" aca="1" ref="S15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
@@ -2302,27 +2313,27 @@
       </c>
       <c r="T15" cm="1">
         <f t="array" aca="1" ref="T15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>37.013511046643494</v>
+        <v>17.204650534085253</v>
       </c>
       <c r="U15" cm="1">
         <f t="array" aca="1" ref="U15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>90.708323763588538</v>
+        <v>10</v>
       </c>
       <c r="V15" cm="1">
         <f t="array" aca="1" ref="V15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>32.649655434629018</v>
+        <v>31.827660925679098</v>
       </c>
       <c r="W15" cm="1">
         <f t="array" aca="1" ref="W15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>77.103826104804938</v>
+        <v>46.518813398452032</v>
       </c>
       <c r="X15" cm="1">
         <f t="array" aca="1" ref="X15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>46.324939287601879</v>
+        <v>26.419689627245813</v>
       </c>
       <c r="Y15" cm="1">
         <f t="array" aca="1" ref="Y15" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E15),INDEX($C$2:$C$21,$E15),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>69.426219830839131</v>
+        <v>41.109609582188931</v>
       </c>
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
@@ -2331,70 +2342,70 @@
       </c>
       <c r="B16">
         <f t="shared" ca="1" si="0"/>
-        <v>76</v>
+        <v>9</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <v>15</v>
       </c>
       <c r="F16" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>25.45584412271571</v>
+        <v>23.769728648009426</v>
       </c>
       <c r="G16" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>47.042533945356304</v>
+        <v>86.95401083331349</v>
       </c>
       <c r="H16" cm="1">
         <f t="array" aca="1" ref="H16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>59.211485372349848</v>
+        <v>33.060550509633082</v>
       </c>
       <c r="I16" cm="1">
         <f t="array" aca="1" ref="I16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>40.36087214122113</v>
+        <v>83.240615086627031</v>
       </c>
       <c r="J16" cm="1">
         <f t="array" aca="1" ref="J16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>63.953107821277925</v>
+        <v>42.941821107167776</v>
       </c>
       <c r="K16" cm="1">
         <f t="array" aca="1" ref="K16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>9.8488578017961039</v>
+        <v>42.01190307520001</v>
       </c>
       <c r="L16" cm="1">
         <f t="array" aca="1" ref="L16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>60.133185513491632</v>
+        <v>110.8873302050329</v>
       </c>
       <c r="M16" cm="1">
         <f t="array" aca="1" ref="M16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>19.697715603592208</v>
+        <v>110.80162453682708</v>
       </c>
       <c r="N16" cm="1">
         <f t="array" aca="1" ref="N16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>95.603347221736954</v>
+        <v>75.325958341065927</v>
       </c>
       <c r="O16" cm="1">
         <f t="array" aca="1" ref="O16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>16.970562748477139</v>
+        <v>29.410882339705484</v>
       </c>
       <c r="P16" cm="1">
         <f t="array" aca="1" ref="P16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>61.1310068623117</v>
+        <v>13.601470508735444</v>
       </c>
       <c r="Q16" cm="1">
         <f t="array" aca="1" ref="Q16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>14.317821063276353</v>
+        <v>60.876925020897694</v>
       </c>
       <c r="R16" cm="1">
         <f t="array" aca="1" ref="R16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>40.26164427839479</v>
+        <v>96.674712308855618</v>
       </c>
       <c r="S16" cm="1">
         <f t="array" aca="1" ref="S16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>37.013511046643494</v>
+        <v>17.204650534085253</v>
       </c>
       <c r="T16" cm="1">
         <f t="array" aca="1" ref="T16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
@@ -2402,23 +2413,23 @@
       </c>
       <c r="U16" cm="1">
         <f t="array" aca="1" ref="U16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>82.619610262939389</v>
+        <v>7.2111025509279782</v>
       </c>
       <c r="V16" cm="1">
         <f t="array" aca="1" ref="V16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>8.2462112512353212</v>
+        <v>33.241540277189323</v>
       </c>
       <c r="W16" cm="1">
         <f t="array" aca="1" ref="W16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>63.28506932918696</v>
+        <v>63.529520697074361</v>
       </c>
       <c r="X16" cm="1">
         <f t="array" aca="1" ref="X16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>16.492422502470642</v>
+        <v>37.12142238654117</v>
       </c>
       <c r="Y16" cm="1">
         <f t="array" aca="1" ref="Y16" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E16),INDEX($C$2:$C$21,$E16),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>33.61547262794322</v>
+        <v>57.77542730261716</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.25">
@@ -2427,74 +2438,74 @@
       </c>
       <c r="B17">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>77</v>
+        <v>29</v>
       </c>
       <c r="E17">
         <v>16</v>
       </c>
       <c r="F17" cm="1">
         <f t="array" aca="1" ref="F17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>89.319650693450427</v>
+        <v>16.763054614240211</v>
       </c>
       <c r="G17" cm="1">
         <f t="array" aca="1" ref="G17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>67.119296778199342</v>
+        <v>79.755877526361658</v>
       </c>
       <c r="H17" cm="1">
         <f t="array" aca="1" ref="H17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>56.320511361314892</v>
+        <v>27.658633371878661</v>
       </c>
       <c r="I17" cm="1">
         <f t="array" aca="1" ref="I17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>42.43819034784589</v>
+        <v>76.400261779656233</v>
       </c>
       <c r="J17" cm="1">
         <f t="array" aca="1" ref="J17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>55.317266743757322</v>
+        <v>36.76955262170047</v>
       </c>
       <c r="K17" cm="1">
         <f t="array" aca="1" ref="K17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>78.492037812761623</v>
+        <v>35.227829907617071</v>
       </c>
       <c r="L17" cm="1">
         <f t="array" aca="1" ref="L17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>69.584481028459209</v>
+        <v>104.01922899156675</v>
       </c>
       <c r="M17" cm="1">
         <f t="array" aca="1" ref="M17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>63.702433234531945</v>
+        <v>104.04326023342406</v>
       </c>
       <c r="N17" cm="1">
         <f t="array" aca="1" ref="N17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>13.038404810405298</v>
+        <v>71.007041904306931</v>
       </c>
       <c r="O17" cm="1">
         <f t="array" aca="1" ref="O17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>86.313382508160345</v>
+        <v>30.479501308256342</v>
       </c>
       <c r="P17" cm="1">
         <f t="array" aca="1" ref="P17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>47.169905660283021</v>
+        <v>17.464249196572979</v>
       </c>
       <c r="Q17" cm="1">
         <f t="array" aca="1" ref="Q17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>95.692214939356489</v>
+        <v>55.731499172371095</v>
       </c>
       <c r="R17" cm="1">
         <f t="array" aca="1" ref="R17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>66.309878600401618</v>
+        <v>89.810912477270818</v>
       </c>
       <c r="S17" cm="1">
         <f t="array" aca="1" ref="S17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>90.708323763588538</v>
+        <v>10</v>
       </c>
       <c r="T17" cm="1">
         <f t="array" aca="1" ref="T17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>82.619610262939389</v>
+        <v>7.2111025509279782</v>
       </c>
       <c r="U17" cm="1">
         <f t="array" aca="1" ref="U17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
@@ -2502,19 +2513,19 @@
       </c>
       <c r="V17" cm="1">
         <f t="array" aca="1" ref="V17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>76.275815302099531</v>
+        <v>31.76476034853718</v>
       </c>
       <c r="W17" cm="1">
         <f t="array" aca="1" ref="W17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>21.095023109728988</v>
+        <v>56.356011214421486</v>
       </c>
       <c r="X17" cm="1">
         <f t="array" aca="1" ref="X17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>67.896980787071826</v>
+        <v>31.780497164141408</v>
       </c>
       <c r="Y17" cm="1">
         <f t="array" aca="1" ref="Y17" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E17),INDEX($C$2:$C$21,$E17),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>76.941536246685374</v>
+        <v>50.695167422546305</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.25">
@@ -2523,78 +2534,78 @@
       </c>
       <c r="B18">
         <f t="shared" ca="1" si="0"/>
-        <v>74</v>
+        <v>41</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="E18">
         <v>17</v>
       </c>
       <c r="F18" cm="1">
         <f t="array" aca="1" ref="F18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>22.360679774997898</v>
+        <v>38.600518131237564</v>
       </c>
       <c r="G18" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>39.204591567825318</v>
+        <v>84.852813742385706</v>
       </c>
       <c r="H18" cm="1">
         <f t="array" aca="1" ref="H18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>58.463663928973865</v>
+        <v>54.037024344425184</v>
       </c>
       <c r="I18" cm="1">
         <f t="array" aca="1" ref="I18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>33.837848631377263</v>
+        <v>69.354163537598808</v>
       </c>
       <c r="J18" cm="1">
         <f t="array" aca="1" ref="J18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>55.731499172371095</v>
+        <v>29.614185789921695</v>
       </c>
       <c r="K18" cm="1">
         <f t="array" aca="1" ref="K18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>13.892443989449804</v>
+        <v>35.014282800023196</v>
       </c>
       <c r="L18" cm="1">
         <f t="array" aca="1" ref="L18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>52.345009313209601</v>
+        <v>95.692214939356489</v>
       </c>
       <c r="M18" cm="1">
         <f t="array" aca="1" ref="M18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>16</v>
+        <v>94.201910808645493</v>
       </c>
       <c r="N18" cm="1">
         <f t="array" aca="1" ref="N18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>89.308454247064432</v>
+        <v>45.880278987817846</v>
       </c>
       <c r="O18" cm="1">
         <f t="array" aca="1" ref="O18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>14.560219778561036</v>
+        <v>11.313708498984761</v>
       </c>
       <c r="P18" cm="1">
         <f t="array" aca="1" ref="P18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>59.135437767890075</v>
+        <v>24.083189157584592</v>
       </c>
       <c r="Q18" cm="1">
         <f t="array" aca="1" ref="Q18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>19.416487838947599</v>
+        <v>36.124783736376884</v>
       </c>
       <c r="R18" cm="1">
         <f t="array" aca="1" ref="R18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>41.146081222881968</v>
+        <v>82.152297594163485</v>
       </c>
       <c r="S18" cm="1">
         <f t="array" aca="1" ref="S18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>32.649655434629018</v>
+        <v>31.827660925679098</v>
       </c>
       <c r="T18" cm="1">
         <f t="array" aca="1" ref="T18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>8.2462112512353212</v>
+        <v>33.241540277189323</v>
       </c>
       <c r="U18" cm="1">
         <f t="array" aca="1" ref="U18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>76.275815302099531</v>
+        <v>31.76476034853718</v>
       </c>
       <c r="V18" cm="1">
         <f t="array" aca="1" ref="V18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
@@ -2602,15 +2613,15 @@
       </c>
       <c r="W18" cm="1">
         <f t="array" aca="1" ref="W18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>57.697486947006624</v>
+        <v>65.030761951556428</v>
       </c>
       <c r="X18" cm="1">
         <f t="array" aca="1" ref="X18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>14.560219778561036</v>
+        <v>57.801384066473702</v>
       </c>
       <c r="Y18" cm="1">
         <f t="array" aca="1" ref="Y18" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E18),INDEX($C$2:$C$21,$E18),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>36.796738985948195</v>
+        <v>62.649820430708338</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.25">
@@ -2619,82 +2630,82 @@
       </c>
       <c r="B19">
         <f t="shared" ca="1" si="0"/>
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>59</v>
+        <v>79</v>
       </c>
       <c r="E19">
         <v>18</v>
       </c>
       <c r="F19" cm="1">
         <f t="array" aca="1" ref="F19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>73.545904032787575</v>
+        <v>39.962482405376171</v>
       </c>
       <c r="G19" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>57.723478758647246</v>
+        <v>23.600847442411894</v>
       </c>
       <c r="H19" cm="1">
         <f t="array" aca="1" ref="H19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>38.327535793473601</v>
+        <v>39.408120990476064</v>
       </c>
       <c r="I19" cm="1">
         <f t="array" aca="1" ref="I19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>24.738633753705962</v>
+        <v>35.227829907617071</v>
       </c>
       <c r="J19" cm="1">
         <f t="array" aca="1" ref="J19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>52.430906915673319</v>
+        <v>36.878177829171548</v>
       </c>
       <c r="K19" cm="1">
         <f t="array" aca="1" ref="K19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>58.258046654518033</v>
+        <v>30.14962686336267</v>
       </c>
       <c r="L19" cm="1">
         <f t="array" aca="1" ref="L19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>63.976558206893252</v>
+        <v>57.723478758647246</v>
       </c>
       <c r="M19" cm="1">
         <f t="array" aca="1" ref="M19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>43.829214001622255</v>
+        <v>59.841457201508724</v>
       </c>
       <c r="N19" cm="1">
         <f t="array" aca="1" ref="N19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>33.301651610693426</v>
+        <v>66.528189513919585</v>
       </c>
       <c r="O19" cm="1">
         <f t="array" aca="1" ref="O19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>69.260378283691168</v>
+        <v>73.246160308919954</v>
       </c>
       <c r="P19" cm="1">
         <f t="array" aca="1" ref="P19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>29.832867780352597</v>
+        <v>70.51950084905593</v>
       </c>
       <c r="Q19" cm="1">
         <f t="array" aca="1" ref="Q19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>76.941536246685374</v>
+        <v>50.219518117958877</v>
       </c>
       <c r="R19" cm="1">
         <f t="array" aca="1" ref="R19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>45.541190146942803</v>
+        <v>45.276925690687087</v>
       </c>
       <c r="S19" cm="1">
         <f t="array" aca="1" ref="S19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>77.103826104804938</v>
+        <v>46.518813398452032</v>
       </c>
       <c r="T19" cm="1">
         <f t="array" aca="1" ref="T19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>63.28506932918696</v>
+        <v>63.529520697074361</v>
       </c>
       <c r="U19" cm="1">
         <f t="array" aca="1" ref="U19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>21.095023109728988</v>
+        <v>56.356011214421486</v>
       </c>
       <c r="V19" cm="1">
         <f t="array" aca="1" ref="V19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>57.697486947006624</v>
+        <v>65.030761951556428</v>
       </c>
       <c r="W19" cm="1">
         <f t="array" aca="1" ref="W19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
@@ -2702,11 +2713,11 @@
       </c>
       <c r="X19" cm="1">
         <f t="array" aca="1" ref="X19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>47.801673610868477</v>
+        <v>38.078865529319543</v>
       </c>
       <c r="Y19" cm="1">
         <f t="array" aca="1" ref="Y19" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E19),INDEX($C$2:$C$21,$E19),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>55.901699437494742</v>
+        <v>7.6157731058639087</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.25">
@@ -2715,86 +2726,86 @@
       </c>
       <c r="B20">
         <f t="shared" ca="1" si="0"/>
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="E20">
         <v>19</v>
       </c>
       <c r="F20" cm="1">
         <f t="array" aca="1" ref="F20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>36.76955262170047</v>
+        <v>19.209372712298546</v>
       </c>
       <c r="G20" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>46.61544808322666</v>
+        <v>60.440052945046304</v>
       </c>
       <c r="H20" cm="1">
         <f t="array" aca="1" ref="H20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>43.931765272977593</v>
+        <v>4.1231056256176606</v>
       </c>
       <c r="I20" cm="1">
         <f t="array" aca="1" ref="I20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>26.92582403567252</v>
+        <v>69.634761434214738</v>
       </c>
       <c r="J20" cm="1">
         <f t="array" aca="1" ref="J20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>59.211485372349848</v>
+        <v>44.384682042344295</v>
       </c>
       <c r="K20" cm="1">
         <f t="array" aca="1" ref="K20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>10.63014581273465</v>
+        <v>37.643060449437421</v>
       </c>
       <c r="L20" cm="1">
         <f t="array" aca="1" ref="L20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>59.464274989274024</v>
+        <v>94.921019800674287</v>
       </c>
       <c r="M20" cm="1">
         <f t="array" aca="1" ref="M20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>4.4721359549995796</v>
+        <v>96.462427918853464</v>
       </c>
       <c r="N20" cm="1">
         <f t="array" aca="1" ref="N20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>80.721744282442259</v>
+        <v>83.570329663104715</v>
       </c>
       <c r="O20" cm="1">
         <f t="array" aca="1" ref="O20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>29.120439557122072</v>
+        <v>60.373835392494321</v>
       </c>
       <c r="P20" cm="1">
         <f t="array" aca="1" ref="P20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>45</v>
+        <v>49.244289008980523</v>
       </c>
       <c r="Q20" cm="1">
         <f t="array" aca="1" ref="Q20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>30.805843601498726</v>
+        <v>65.787536813594102</v>
       </c>
       <c r="R20" cm="1">
         <f t="array" aca="1" ref="R20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>26.92582403567252</v>
+        <v>81.60882305241266</v>
       </c>
       <c r="S20" cm="1">
         <f t="array" aca="1" ref="S20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>46.324939287601879</v>
+        <v>26.419689627245813</v>
       </c>
       <c r="T20" cm="1">
         <f t="array" aca="1" ref="T20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>16.492422502470642</v>
+        <v>37.12142238654117</v>
       </c>
       <c r="U20" cm="1">
         <f t="array" aca="1" ref="U20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>67.896980787071826</v>
+        <v>31.780497164141408</v>
       </c>
       <c r="V20" cm="1">
         <f t="array" aca="1" ref="V20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>14.560219778561036</v>
+        <v>57.801384066473702</v>
       </c>
       <c r="W20" cm="1">
         <f t="array" aca="1" ref="W20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>47.801673610868477</v>
+        <v>38.078865529319543</v>
       </c>
       <c r="X20" cm="1">
         <f t="array" aca="1" ref="X20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
@@ -2802,7 +2813,7 @@
       </c>
       <c r="Y20" cm="1">
         <f t="array" aca="1" ref="Y20" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E20),INDEX($C$2:$C$21,$E20),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
-        <v>24.698178070456937</v>
+        <v>30.528675044947494</v>
       </c>
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.25">
@@ -2811,90 +2822,90 @@
       </c>
       <c r="B21">
         <f t="shared" ca="1" si="0"/>
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>76</v>
       </c>
       <c r="E21">
         <v>20</v>
       </c>
       <c r="F21" cm="1">
         <f t="array" aca="1" ref="F21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,F$1),INDEX($C$2:$C$21,F$1))</f>
-        <v>58.600341295934449</v>
+        <v>34.014702703389901</v>
       </c>
       <c r="G21" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,G$1),INDEX($C$2:$C$21,G$1))</f>
-        <v>71.112586790244109</v>
+        <v>30.413812651491099</v>
       </c>
       <c r="H21" cm="1">
         <f t="array" aca="1" ref="H21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,H$1),INDEX($C$2:$C$21,H$1))</f>
-        <v>32.310988842807021</v>
+        <v>32.015621187164243</v>
       </c>
       <c r="I21" cm="1">
         <f t="array" aca="1" ref="I21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,I$1),INDEX($C$2:$C$21,I$1))</f>
-        <v>44.011362169330773</v>
+        <v>42.01190307520001</v>
       </c>
       <c r="J21" cm="1">
         <f t="array" aca="1" ref="J21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,J$1),INDEX($C$2:$C$21,J$1))</f>
-        <v>82</v>
+        <v>36.249137920783717</v>
       </c>
       <c r="K21" cm="1">
         <f t="array" aca="1" ref="K21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,K$1),INDEX($C$2:$C$21,K$1))</f>
-        <v>23.853720883753127</v>
+        <v>28.792360097775937</v>
       </c>
       <c r="L21" cm="1">
         <f t="array" aca="1" ref="L21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,L$1),INDEX($C$2:$C$21,L$1))</f>
-        <v>83.773504164502995</v>
+        <v>65.253352404301808</v>
       </c>
       <c r="M21" cm="1">
         <f t="array" aca="1" ref="M21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,M$1),INDEX($C$2:$C$21,M$1))</f>
-        <v>27.313000567495326</v>
+        <v>67.268120235368556</v>
       </c>
       <c r="N21" cm="1">
         <f t="array" aca="1" ref="N21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,N$1),INDEX($C$2:$C$21,N$1))</f>
-        <v>88.509886453435243</v>
+        <v>69.426219830839131</v>
       </c>
       <c r="O21" cm="1">
         <f t="array" aca="1" ref="O21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,O$1),INDEX($C$2:$C$21,O$1))</f>
-        <v>50.219518117958877</v>
+        <v>70.007142492748557</v>
       </c>
       <c r="P21" cm="1">
         <f t="array" aca="1" ref="P21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,P$1),INDEX($C$2:$C$21,P$1))</f>
-        <v>38.275318418009277</v>
+        <v>65.73431371817918</v>
       </c>
       <c r="Q21" cm="1">
         <f t="array" aca="1" ref="Q21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,Q$1),INDEX($C$2:$C$21,Q$1))</f>
-        <v>45.221676218380054</v>
+        <v>52.345009313209601</v>
       </c>
       <c r="R21" cm="1">
         <f t="array" aca="1" ref="R21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,R$1),INDEX($C$2:$C$21,R$1))</f>
-        <v>12.206555615733702</v>
+        <v>52.611785751863621</v>
       </c>
       <c r="S21" cm="1">
         <f t="array" aca="1" ref="S21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,S$1),INDEX($C$2:$C$21,S$1))</f>
-        <v>69.426219830839131</v>
+        <v>41.109609582188931</v>
       </c>
       <c r="T21" cm="1">
         <f t="array" aca="1" ref="T21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,T$1),INDEX($C$2:$C$21,T$1))</f>
-        <v>33.61547262794322</v>
+        <v>57.77542730261716</v>
       </c>
       <c r="U21" cm="1">
         <f t="array" aca="1" ref="U21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,U$1),INDEX($C$2:$C$21,U$1))</f>
-        <v>76.941536246685374</v>
+        <v>50.695167422546305</v>
       </c>
       <c r="V21" cm="1">
         <f t="array" aca="1" ref="V21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,V$1),INDEX($C$2:$C$21,V$1))</f>
-        <v>36.796738985948195</v>
+        <v>62.649820430708338</v>
       </c>
       <c r="W21" cm="1">
         <f t="array" aca="1" ref="W21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,W$1),INDEX($C$2:$C$21,W$1))</f>
-        <v>55.901699437494742</v>
+        <v>7.6157731058639087</v>
       </c>
       <c r="X21" cm="1">
         <f t="array" aca="1" ref="X21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,X$1),INDEX($C$2:$C$21,X$1))</f>
-        <v>24.698178070456937</v>
+        <v>30.528675044947494</v>
       </c>
       <c r="Y21" cm="1">
         <f t="array" aca="1" ref="Y21" ca="1">DistEuclidea(INDEX($B$2:$B$21,$E21),INDEX($C$2:$C$21,$E21),INDEX($B$2:$B$21,Y$1),INDEX($C$2:$C$21,Y$1))</f>
@@ -2907,11 +2918,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:T20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>

</xml_diff>